<commit_message>
Fixed compatibility for simulation
</commit_message>
<xml_diff>
--- a/Simulasi/Simulasi Gantry ICA/Variasi ICA/result.xlsx
+++ b/Simulasi/Simulasi Gantry ICA/Variasi ICA/result.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -618,7 +618,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>3.615</v>
+        <v>3.62</v>
       </c>
       <c r="C6" t="n">
         <v>5.56</v>
@@ -627,10 +627,10 @@
         <v>0.003</v>
       </c>
       <c r="E6" t="n">
-        <v>3.98</v>
+        <v>4.315</v>
       </c>
       <c r="F6" t="n">
-        <v>4.81</v>
+        <v>5.145</v>
       </c>
       <c r="G6" t="n">
         <v>0.003</v>
@@ -639,7 +639,7 @@
         <v>0.65</v>
       </c>
       <c r="I6" t="n">
-        <v>3.88</v>
+        <v>3.885</v>
       </c>
       <c r="J6" t="n">
         <v>0.122</v>

</xml_diff>